<commit_message>
Saving analysis for the paper
</commit_message>
<xml_diff>
--- a/raw-data/wb_data.xlsx
+++ b/raw-data/wb_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabe/Desktop/Projects/Gov94Analysis/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E9C920-58F1-1046-A7AE-45B31B645FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A249C0-78BE-B54A-B763-B596EC0563E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="3020" windowWidth="25640" windowHeight="14040" xr2:uid="{33E7C126-37A0-6D4E-9BBF-0058AD324F0A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$265</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$265</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="538">
   <si>
     <t>Aruba</t>
   </si>
@@ -1647,6 +1647,9 @@
   </si>
   <si>
     <t>people_per_sq_km</t>
+  </si>
+  <si>
+    <t>informal_sector</t>
   </si>
 </sst>
 </file>
@@ -1689,9 +1692,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2006,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D6A769-183A-1348-AF8E-A43228ED1088}">
-  <dimension ref="A1:I265"/>
+  <dimension ref="A1:J265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2017,9 +2021,10 @@
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="37.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>531</v>
       </c>
@@ -2044,11 +2049,14 @@
       <c r="H1" t="s">
         <v>536</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="J1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2059,11 +2067,11 @@
       <c r="H2" s="1">
         <v>585.36666700000001</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2085,11 +2093,11 @@
       <c r="H3" s="1">
         <v>55.595993</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2111,11 +2119,11 @@
       <c r="H4" s="1">
         <v>23.9165381</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2140,11 +2148,11 @@
       <c r="H5" s="1">
         <v>104.870693</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2166,11 +2174,11 @@
       <c r="H6" s="1">
         <v>163.83191500000001</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2192,11 +2200,11 @@
       <c r="H7" s="1">
         <v>36.6698041</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2218,11 +2226,11 @@
       <c r="H8" s="1">
         <v>133.584948</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2247,11 +2255,14 @@
       <c r="H9" s="1">
         <v>16.0941908</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="2">
+        <v>47.930000305175803</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2276,11 +2287,14 @@
       <c r="H10" s="1">
         <v>103.43551100000001</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" s="2">
+        <v>24.75</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2294,11 +2308,11 @@
       <c r="H11" s="1">
         <v>278.10000000000002</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2320,11 +2334,11 @@
       <c r="H12" s="1">
         <v>216.877273</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2346,11 +2360,11 @@
       <c r="H13" s="1">
         <v>3.1983614199999999</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2375,11 +2389,11 @@
       <c r="H14" s="1">
         <v>106.607445</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2401,11 +2415,11 @@
       <c r="H15" s="1">
         <v>119.19720599999999</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2427,11 +2441,11 @@
       <c r="H16" s="1">
         <v>421.61308400000001</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2456,11 +2470,11 @@
       <c r="H17" s="1">
         <v>375.66572000000002</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2482,11 +2496,11 @@
       <c r="H18" s="1">
         <v>99.106101499999994</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2508,11 +2522,11 @@
       <c r="H19" s="1">
         <v>70.150891799999997</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2534,11 +2548,14 @@
       <c r="H20" s="1">
         <v>1226.6312700000001</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="2">
+        <v>91.300003051757798</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2563,11 +2580,11 @@
       <c r="H21" s="1">
         <v>65.180057099999999</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2589,11 +2606,11 @@
       <c r="H22" s="1">
         <v>1920.4035200000001</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2615,11 +2632,11 @@
       <c r="H23" s="1">
         <v>38.137962000000002</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2641,11 +2658,14 @@
       <c r="H24" s="1">
         <v>65.459511699999993</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="2">
+        <v>19.110000610351602</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2670,11 +2690,11 @@
       <c r="H25" s="1">
         <v>46.792242100000003</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2696,11 +2716,11 @@
       <c r="H26" s="1">
         <v>16.4738711</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2711,11 +2731,11 @@
       <c r="H27" s="1">
         <v>1182.8518300000001</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2740,11 +2760,14 @@
       <c r="H28" s="1">
         <v>10.3321831</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="2">
+        <v>71.510002136230497</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2769,11 +2792,14 @@
       <c r="H29" s="1">
         <v>24.866038499999998</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2">
+        <v>38.2700004577637</v>
+      </c>
+      <c r="J29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2795,11 +2821,11 @@
       <c r="H30" s="1">
         <v>665.65814</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2821,11 +2847,14 @@
       <c r="H31" s="1">
         <v>80.545161300000004</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="2">
+        <v>32.360000610351598</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2850,11 +2879,11 @@
       <c r="H32" s="1">
         <v>19.5461414</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2876,11 +2905,11 @@
       <c r="H33" s="1">
         <v>3.89096748</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2902,11 +2931,11 @@
       <c r="H34" s="1">
         <v>7.3774888399999998</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2928,11 +2957,11 @@
       <c r="H35" s="1">
         <v>4.0182798499999999</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2954,11 +2983,11 @@
       <c r="H36" s="1">
         <v>92.971794900000006</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2983,11 +3012,11 @@
       <c r="H37" s="1">
         <v>213.88399100000001</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2998,11 +3027,11 @@
       <c r="H38" s="1">
         <v>851.84346700000003</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -3027,11 +3056,14 @@
       <c r="H39" s="1">
         <v>24.8414839</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="2">
+        <v>27.680000305175799</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -3053,11 +3085,11 @@
       <c r="H40" s="1">
         <v>147.67405099999999</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -3079,11 +3111,14 @@
       <c r="H41" s="1">
         <v>76.847386799999995</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I41" s="2">
+        <v>84.830001831054702</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -3105,11 +3140,11 @@
       <c r="H42" s="1">
         <v>51.968532500000002</v>
       </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -3131,11 +3166,11 @@
       <c r="H43" s="1">
         <v>35.905147200000002</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3157,11 +3192,11 @@
       <c r="H44" s="1">
         <v>14.9654524</v>
       </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -3186,11 +3221,14 @@
       <c r="H45" s="1">
         <v>44.074868000000002</v>
       </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="2">
+        <v>56.7700004577637</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -3212,11 +3250,11 @@
       <c r="H46" s="1">
         <v>437.34120000000001</v>
       </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -3238,11 +3276,11 @@
       <c r="H47" s="1">
         <v>133.37394499999999</v>
       </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -3267,11 +3305,14 @@
       <c r="H48" s="1">
         <v>96.943870000000004</v>
       </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="2">
+        <v>35.450000762939503</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -3293,11 +3334,11 @@
       <c r="H49" s="1">
         <v>18.0683957</v>
       </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -3319,11 +3360,11 @@
       <c r="H50" s="1">
         <v>109.010373</v>
       </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -3334,11 +3375,11 @@
       <c r="H51" s="1">
         <v>360.75450499999999</v>
       </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -3349,11 +3390,11 @@
       <c r="H52" s="1">
         <v>264.09166699999997</v>
       </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -3378,11 +3419,11 @@
       <c r="H53" s="1">
         <v>127.670996</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -3407,11 +3448,11 @@
       <c r="H54" s="1">
         <v>137.19810899999999</v>
       </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -3433,11 +3474,11 @@
       <c r="H55" s="1">
         <v>236.595495</v>
       </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -3459,11 +3500,11 @@
       <c r="H56" s="1">
         <v>40.728947400000003</v>
       </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -3485,11 +3526,11 @@
       <c r="H57" s="1">
         <v>95.277333299999995</v>
       </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -3514,11 +3555,11 @@
       <c r="H58" s="1">
         <v>137.294118</v>
       </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -3543,11 +3584,14 @@
       <c r="H59" s="1">
         <v>217.618112</v>
       </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I59" s="2">
+        <v>53.889999389648402</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -3569,11 +3613,11 @@
       <c r="H60" s="1">
         <v>17.377714600000001</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -3595,11 +3639,11 @@
       <c r="H61" s="1">
         <v>129.96233799999999</v>
       </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -3621,11 +3665,11 @@
       <c r="H62" s="1">
         <v>96.871226399999998</v>
       </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -3647,11 +3691,11 @@
       <c r="H63" s="1">
         <v>94.856985199999997</v>
       </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -3673,11 +3717,11 @@
       <c r="H64" s="1">
         <v>18.376258499999999</v>
       </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -3699,11 +3743,11 @@
       <c r="H65" s="1">
         <v>33.3606549</v>
       </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -3728,11 +3772,14 @@
       <c r="H66" s="1">
         <v>67.584800299999998</v>
       </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I66" s="2">
+        <v>64.849998474121094</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -3757,11 +3804,14 @@
       <c r="H67" s="1">
         <v>96.883412500000006</v>
       </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I67" s="2">
+        <v>52.889999389648402</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -3783,11 +3833,11 @@
       <c r="H68" s="1">
         <v>127.351286</v>
       </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3804,11 +3854,11 @@
         <v>17.653454199999999</v>
       </c>
       <c r="H69" s="1"/>
-      <c r="I69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -3833,11 +3883,11 @@
       <c r="H70" s="1">
         <v>93.267804400000003</v>
       </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -3862,11 +3912,11 @@
       <c r="H71" s="1">
         <v>30.3055901</v>
       </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -3888,11 +3938,11 @@
       <c r="H72" s="1">
         <v>106.400024</v>
       </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -3914,11 +3964,11 @@
       <c r="H73" s="1">
         <v>105.252298</v>
       </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -3940,11 +3990,11 @@
       <c r="H74" s="1">
         <v>38.977770499999998</v>
       </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -3969,11 +4019,11 @@
       <c r="H75" s="1">
         <v>18.1244908</v>
       </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -3995,11 +4045,11 @@
       <c r="H76" s="1">
         <v>48.027312500000001</v>
       </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -4024,11 +4074,11 @@
       <c r="H77" s="1">
         <v>122.115405</v>
       </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -4039,11 +4089,11 @@
       <c r="H78" s="1">
         <v>34.621058699999999</v>
       </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -4065,11 +4115,11 @@
       <c r="H79" s="1">
         <v>159.22714300000001</v>
       </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -4094,11 +4144,11 @@
       <c r="H80" s="1">
         <v>8.0134396700000003</v>
       </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -4120,11 +4170,11 @@
       <c r="H81" s="1">
         <v>273.04947299999998</v>
       </c>
-      <c r="I81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -4149,11 +4199,11 @@
       <c r="H82" s="1">
         <v>65.222785999999999</v>
       </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -4175,11 +4225,11 @@
       <c r="H83" s="1">
         <v>127.983963</v>
       </c>
-      <c r="I83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -4190,11 +4240,11 @@
       <c r="H84" s="1">
         <v>3372.8</v>
       </c>
-      <c r="I84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -4216,11 +4266,11 @@
       <c r="H85" s="1">
         <v>49.1109352</v>
       </c>
-      <c r="I85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -4242,11 +4292,11 @@
       <c r="H86" s="1">
         <v>218.764229</v>
       </c>
-      <c r="I86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -4268,11 +4318,11 @@
       <c r="H87" s="1">
         <v>65.012304400000005</v>
       </c>
-      <c r="I87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -4294,11 +4344,11 @@
       <c r="H88" s="1">
         <v>44.991123000000002</v>
       </c>
-      <c r="I88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -4323,11 +4373,11 @@
       <c r="H89" s="1">
         <v>83.434282400000001</v>
       </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -4349,11 +4399,11 @@
       <c r="H90" s="1">
         <v>326.10000000000002</v>
       </c>
-      <c r="I90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -4367,11 +4417,11 @@
       <c r="H91" s="1">
         <v>0.13685224000000001</v>
       </c>
-      <c r="I91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -4393,11 +4443,14 @@
       <c r="H92" s="1">
         <v>157.84747999999999</v>
       </c>
-      <c r="I92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I92" s="2">
+        <v>72.779998779296903</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -4411,11 +4464,11 @@
       <c r="H93" s="1">
         <v>304.22407399999997</v>
       </c>
-      <c r="I93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -4437,11 +4490,11 @@
       <c r="H94" s="1">
         <v>3.9381305599999998</v>
       </c>
-      <c r="I94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -4463,11 +4516,11 @@
       <c r="H95" s="1">
         <v>34.269863999999998</v>
       </c>
-      <c r="I95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -4481,11 +4534,11 @@
       <c r="H96" s="1">
         <v>7039.7142899999999</v>
       </c>
-      <c r="I96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -4510,11 +4563,14 @@
       <c r="H97" s="1">
         <v>84.270381599999993</v>
       </c>
-      <c r="I97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I97" s="2">
+        <v>75.559997558593807</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -4536,11 +4592,11 @@
       <c r="H98" s="1">
         <v>43.680036299999998</v>
       </c>
-      <c r="I98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -4565,11 +4621,11 @@
       <c r="H99" s="1">
         <v>73.704985699999995</v>
       </c>
-      <c r="I99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -4591,11 +4647,14 @@
       <c r="H100" s="1">
         <v>398.48933199999999</v>
       </c>
-      <c r="I100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I100" s="2">
+        <v>88.120002746582003</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -4620,11 +4679,11 @@
       <c r="H101" s="1">
         <v>108.11848000000001</v>
       </c>
-      <c r="I101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -4646,11 +4705,11 @@
       <c r="H102" s="1">
         <v>68.192583999999997</v>
       </c>
-      <c r="I102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -4672,11 +4731,11 @@
       <c r="H103" s="1">
         <v>67.870329400000003</v>
       </c>
-      <c r="I103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -4698,11 +4757,11 @@
       <c r="H104" s="1">
         <v>66.937265800000006</v>
       </c>
-      <c r="I104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -4724,11 +4783,11 @@
       <c r="H105" s="1">
         <v>91.259624500000001</v>
       </c>
-      <c r="I105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -4753,11 +4812,14 @@
       <c r="H106" s="1">
         <v>146.08648099999999</v>
       </c>
-      <c r="I106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I106" s="2">
+        <v>78.529998779296903</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -4779,11 +4841,11 @@
       <c r="H107" s="1">
         <v>58.892063800000003</v>
       </c>
-      <c r="I107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -4794,11 +4856,11 @@
       <c r="H108" s="1">
         <v>146.66315800000001</v>
       </c>
-      <c r="I108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -4820,11 +4882,11 @@
       <c r="H109" s="1">
         <v>450.24328600000001</v>
       </c>
-      <c r="I109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>216</v>
       </c>
@@ -4833,11 +4895,11 @@
       </c>
       <c r="F110" s="1"/>
       <c r="H110" s="1"/>
-      <c r="I110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>218</v>
       </c>
@@ -4859,11 +4921,11 @@
       <c r="H111" s="1">
         <v>69.783539000000005</v>
       </c>
-      <c r="I111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -4885,11 +4947,11 @@
       <c r="H112" s="1">
         <v>49.530901399999998</v>
       </c>
-      <c r="I112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -4911,11 +4973,11 @@
       <c r="H113" s="1">
         <v>86.501631599999996</v>
       </c>
-      <c r="I113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>224</v>
       </c>
@@ -4937,11 +4999,11 @@
       <c r="H114" s="1">
         <v>3.4254364100000001</v>
       </c>
-      <c r="I114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>226</v>
       </c>
@@ -4963,11 +5025,11 @@
       <c r="H115" s="1">
         <v>402.647874</v>
       </c>
-      <c r="I115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>228</v>
       </c>
@@ -4992,11 +5054,11 @@
       <c r="H116" s="1">
         <v>205.809169</v>
       </c>
-      <c r="I116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>230</v>
       </c>
@@ -5018,11 +5080,11 @@
       <c r="H117" s="1">
         <v>269.70018499999998</v>
       </c>
-      <c r="I117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -5044,11 +5106,11 @@
       <c r="H118" s="1">
         <v>110.150631</v>
       </c>
-      <c r="I118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>234</v>
       </c>
@@ -5070,11 +5132,11 @@
       <c r="H119" s="1">
         <v>347.77758699999998</v>
       </c>
-      <c r="I119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>236</v>
       </c>
@@ -5099,11 +5161,11 @@
       <c r="H120" s="1">
         <v>6.6814001599999999</v>
       </c>
-      <c r="I120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>238</v>
       </c>
@@ -5125,11 +5187,11 @@
       <c r="H121" s="1">
         <v>88.240982900000006</v>
       </c>
-      <c r="I121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>240</v>
       </c>
@@ -5154,11 +5216,11 @@
       <c r="H122" s="1">
         <v>32.315954099999999</v>
       </c>
-      <c r="I122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>242</v>
       </c>
@@ -5180,11 +5242,11 @@
       <c r="H123" s="1">
         <v>90.694618199999994</v>
       </c>
-      <c r="I123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>244</v>
       </c>
@@ -5206,11 +5268,11 @@
       <c r="H124" s="1">
         <v>140.935802</v>
       </c>
-      <c r="I124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>246</v>
       </c>
@@ -5232,11 +5294,11 @@
       <c r="H125" s="1">
         <v>200.17307700000001</v>
       </c>
-      <c r="I125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>248</v>
       </c>
@@ -5258,11 +5320,11 @@
       <c r="H126" s="1">
         <v>527.91801099999998</v>
       </c>
-      <c r="I126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -5284,11 +5346,11 @@
       <c r="H127" s="1">
         <v>227.61487099999999</v>
       </c>
-      <c r="I127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>252</v>
       </c>
@@ -5310,11 +5372,11 @@
       <c r="H128" s="1">
         <v>31.718614200000001</v>
       </c>
-      <c r="I128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>254</v>
       </c>
@@ -5336,11 +5398,14 @@
       <c r="H129" s="1">
         <v>30.125801599999999</v>
       </c>
-      <c r="I129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I129" s="2">
+        <v>75.5</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -5362,11 +5427,11 @@
       <c r="H130" s="1">
         <v>665.87223900000004</v>
       </c>
-      <c r="I130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>258</v>
       </c>
@@ -5388,11 +5453,11 @@
       <c r="H131" s="1">
         <v>48.818812299999998</v>
       </c>
-      <c r="I131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>260</v>
       </c>
@@ -5406,11 +5471,11 @@
       <c r="H132" s="1">
         <v>3.7400252300000001</v>
       </c>
-      <c r="I132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>262</v>
       </c>
@@ -5432,11 +5497,11 @@
       <c r="H133" s="1">
         <v>296.64754099999999</v>
       </c>
-      <c r="I133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>264</v>
       </c>
@@ -5458,11 +5523,11 @@
       <c r="H134" s="1">
         <v>31.706220900000002</v>
       </c>
-      <c r="I134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>266</v>
       </c>
@@ -5484,11 +5549,11 @@
       <c r="H135" s="1">
         <v>55.5297415</v>
       </c>
-      <c r="I135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>268</v>
       </c>
@@ -5510,11 +5575,11 @@
       <c r="H136" s="1">
         <v>50.357548700000002</v>
       </c>
-      <c r="I136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>270</v>
       </c>
@@ -5525,11 +5590,11 @@
       <c r="H137" s="1">
         <v>236.25</v>
       </c>
-      <c r="I137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>272</v>
       </c>
@@ -5551,11 +5616,14 @@
       <c r="H138" s="1">
         <v>341.95503100000002</v>
       </c>
-      <c r="I138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I138" s="2">
+        <v>64.480003356933594</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>274</v>
       </c>
@@ -5577,11 +5645,11 @@
       <c r="H139" s="1">
         <v>148.02188699999999</v>
       </c>
-      <c r="I139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>276</v>
       </c>
@@ -5603,11 +5671,11 @@
       <c r="H140" s="1">
         <v>68.394054199999999</v>
       </c>
-      <c r="I140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -5632,11 +5700,11 @@
       <c r="H141" s="1">
         <v>68.887088300000002</v>
       </c>
-      <c r="I141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -5658,11 +5726,11 @@
       <c r="H142" s="1">
         <v>51.131386800000001</v>
       </c>
-      <c r="I142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>282</v>
       </c>
@@ -5687,11 +5755,11 @@
       <c r="H143" s="1">
         <v>45.151861599999997</v>
       </c>
-      <c r="I143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>284</v>
       </c>
@@ -5716,11 +5784,11 @@
       <c r="H144" s="1">
         <v>245.40576100000001</v>
       </c>
-      <c r="I144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>286</v>
       </c>
@@ -5745,11 +5813,11 @@
       <c r="H145" s="1">
         <v>31.235895800000002</v>
       </c>
-      <c r="I145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>288</v>
       </c>
@@ -5763,11 +5831,11 @@
       <c r="H146" s="1">
         <v>20479.77</v>
       </c>
-      <c r="I146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>290</v>
       </c>
@@ -5778,11 +5846,11 @@
       <c r="H147" s="1">
         <v>672.05882399999996</v>
       </c>
-      <c r="I147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>292</v>
       </c>
@@ -5804,11 +5872,11 @@
       <c r="H148" s="1">
         <v>79.725059400000006</v>
       </c>
-      <c r="I148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>294</v>
       </c>
@@ -5830,11 +5898,11 @@
       <c r="H149" s="1">
         <v>19196</v>
       </c>
-      <c r="I149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>296</v>
       </c>
@@ -5859,11 +5927,11 @@
       <c r="H150" s="1">
         <v>123.635211</v>
       </c>
-      <c r="I150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>298</v>
       </c>
@@ -5885,11 +5953,11 @@
       <c r="H151" s="1">
         <v>43.9507391</v>
       </c>
-      <c r="I151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>300</v>
       </c>
@@ -5911,11 +5979,11 @@
       <c r="H152" s="1">
         <v>1654.6733300000001</v>
       </c>
-      <c r="I152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -5937,11 +6005,11 @@
       <c r="H153" s="1">
         <v>39.315415899999998</v>
       </c>
-      <c r="I153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>304</v>
       </c>
@@ -5963,11 +6031,14 @@
       <c r="H154" s="1">
         <v>64.187517200000002</v>
       </c>
-      <c r="I154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I154" s="2">
+        <v>58.79</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>306</v>
       </c>
@@ -5989,11 +6060,11 @@
       <c r="H155" s="1">
         <v>322.544444</v>
       </c>
-      <c r="I155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>308</v>
       </c>
@@ -6015,11 +6086,11 @@
       <c r="H156" s="1">
         <v>71.528344200000006</v>
       </c>
-      <c r="I156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>310</v>
       </c>
@@ -6044,11 +6115,11 @@
       <c r="H157" s="1">
         <v>82.553370299999997</v>
       </c>
-      <c r="I157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>312</v>
       </c>
@@ -6070,11 +6141,14 @@
       <c r="H158" s="1">
         <v>15.1717306</v>
       </c>
-      <c r="I158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I158" s="2">
+        <v>90.620002746582003</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>314</v>
       </c>
@@ -6099,11 +6173,11 @@
       <c r="H159" s="1">
         <v>1462.4968799999999</v>
       </c>
-      <c r="I159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>316</v>
       </c>
@@ -6128,11 +6202,14 @@
       <c r="H160" s="1">
         <v>81.739727099999996</v>
       </c>
-      <c r="I160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I160" s="2">
+        <v>77.739997863769503</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>318</v>
       </c>
@@ -6151,11 +6228,11 @@
       <c r="H161" s="1">
         <v>43.576312899999998</v>
       </c>
-      <c r="I161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>320</v>
       </c>
@@ -6177,11 +6254,11 @@
       <c r="H162" s="1">
         <v>46.273085500000001</v>
       </c>
-      <c r="I162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>322</v>
       </c>
@@ -6203,11 +6280,14 @@
       <c r="H163" s="1">
         <v>2.0042862800000001</v>
       </c>
-      <c r="I163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I163" s="2">
+        <v>32.490001678466797</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>324</v>
       </c>
@@ -6221,11 +6301,11 @@
       <c r="H164" s="1">
         <v>122.96087</v>
       </c>
-      <c r="I164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>326</v>
       </c>
@@ -6247,11 +6327,11 @@
       <c r="H165" s="1">
         <v>36.431505100000003</v>
       </c>
-      <c r="I165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>328</v>
       </c>
@@ -6273,11 +6353,14 @@
       <c r="H166" s="1">
         <v>4.1550150400000003</v>
       </c>
-      <c r="I166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I166" s="2">
+        <v>90.029998779296903</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -6302,11 +6385,14 @@
       <c r="H167" s="1">
         <v>622.96206900000004</v>
       </c>
-      <c r="I167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I167" s="2">
+        <v>52.169998168945298</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>332</v>
       </c>
@@ -6328,11 +6414,11 @@
       <c r="H168" s="1">
         <v>187.42320699999999</v>
       </c>
-      <c r="I168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>334</v>
       </c>
@@ -6354,11 +6440,11 @@
       <c r="H169" s="1">
         <v>94.673650899999998</v>
       </c>
-      <c r="I169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>336</v>
       </c>
@@ -6380,11 +6466,11 @@
       <c r="H170" s="1">
         <v>19.831784500000001</v>
       </c>
-      <c r="I170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -6406,11 +6492,11 @@
       <c r="H171" s="1">
         <v>2.9182948899999999</v>
       </c>
-      <c r="I171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>340</v>
       </c>
@@ -6421,11 +6507,11 @@
       <c r="H172" s="1">
         <v>15.336433299999999</v>
       </c>
-      <c r="I172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>342</v>
       </c>
@@ -6447,11 +6533,14 @@
       <c r="H173" s="1">
         <v>17.054134399999999</v>
       </c>
-      <c r="I173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I173" s="2">
+        <v>73.410003662109403</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>344</v>
       </c>
@@ -6473,11 +6562,11 @@
       <c r="H174" s="1">
         <v>209.57355999999999</v>
       </c>
-      <c r="I174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>346</v>
       </c>
@@ -6499,11 +6588,14 @@
       <c r="H175" s="1">
         <v>53.056797400000001</v>
       </c>
-      <c r="I175">
+      <c r="I175" s="2">
+        <v>74.910003662109403</v>
+      </c>
+      <c r="J175">
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>348</v>
       </c>
@@ -6528,11 +6620,11 @@
       <c r="H176" s="1">
         <v>508.497952</v>
       </c>
-      <c r="I176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -6557,11 +6649,11 @@
       <c r="H177" s="1">
         <v>14.452575899999999</v>
       </c>
-      <c r="I177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>352</v>
       </c>
@@ -6583,11 +6675,14 @@
       <c r="H178" s="1">
         <v>192.72496699999999</v>
       </c>
-      <c r="I178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I178" s="2">
+        <v>77.620002746582003</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>354</v>
       </c>
@@ -6609,11 +6704,11 @@
       <c r="H179" s="1">
         <v>643.79999999999995</v>
       </c>
-      <c r="I179">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -6635,11 +6730,11 @@
       <c r="H180" s="1">
         <v>18.206296800000001</v>
       </c>
-      <c r="I180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>358</v>
       </c>
@@ -6661,11 +6756,11 @@
       <c r="H181" s="1">
         <v>37.597388799999997</v>
       </c>
-      <c r="I181">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>360</v>
       </c>
@@ -6687,11 +6782,11 @@
       <c r="H182" s="1">
         <v>15.0757189</v>
       </c>
-      <c r="I182">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -6713,11 +6808,11 @@
       <c r="H183" s="1">
         <v>14.8383004</v>
       </c>
-      <c r="I183">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>364</v>
       </c>
@@ -6739,11 +6834,11 @@
       <c r="H184" s="1">
         <v>269.68748199999999</v>
       </c>
-      <c r="I184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>366</v>
       </c>
@@ -6768,11 +6863,14 @@
       <c r="H185" s="1">
         <v>55.243085800000003</v>
       </c>
-      <c r="I185">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I185" s="2">
+        <v>42.700000762939503</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>368</v>
       </c>
@@ -6797,11 +6895,14 @@
       <c r="H186" s="1">
         <v>24.565857000000001</v>
       </c>
-      <c r="I186">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I186" s="2">
+        <v>59.009998321533203</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>370</v>
       </c>
@@ -6823,11 +6924,11 @@
       <c r="H187" s="1">
         <v>352.729195</v>
       </c>
-      <c r="I187">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>372</v>
       </c>
@@ -6849,11 +6950,11 @@
       <c r="H188" s="1">
         <v>38.713043499999998</v>
       </c>
-      <c r="I188">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>374</v>
       </c>
@@ -6875,11 +6976,11 @@
       <c r="H189" s="1">
         <v>18.6327541</v>
       </c>
-      <c r="I189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>376</v>
       </c>
@@ -6904,11 +7005,11 @@
       <c r="H190" s="1">
         <v>124.02373</v>
       </c>
-      <c r="I190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>378</v>
       </c>
@@ -6930,11 +7031,11 @@
       <c r="H191" s="1">
         <v>50.283640400000003</v>
       </c>
-      <c r="I191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>380</v>
       </c>
@@ -6948,11 +7049,14 @@
       <c r="H192" s="1">
         <v>374.85918800000002</v>
       </c>
-      <c r="I192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I192" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>382</v>
       </c>
@@ -6963,11 +7067,11 @@
       <c r="H193" s="1">
         <v>211.19495900000001</v>
       </c>
-      <c r="I193">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>384</v>
       </c>
@@ -6992,11 +7096,11 @@
       <c r="H194" s="1">
         <v>112.441821</v>
       </c>
-      <c r="I194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -7021,11 +7125,14 @@
       <c r="H195" s="1">
         <v>17.2843242</v>
       </c>
-      <c r="I195">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I195" s="2">
+        <v>65.419998168945298</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>388</v>
       </c>
@@ -7039,11 +7146,14 @@
       <c r="H196" s="1">
         <v>740.00083099999995</v>
       </c>
-      <c r="I196">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I196" s="2">
+        <v>51.930000305175803</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>390</v>
       </c>
@@ -7065,11 +7175,11 @@
       <c r="H197" s="1">
         <v>37.727196300000003</v>
       </c>
-      <c r="I197">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>392</v>
       </c>
@@ -7091,11 +7201,11 @@
       <c r="H198" s="1">
         <v>35.141603199999999</v>
       </c>
-      <c r="I198">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>394</v>
       </c>
@@ -7106,11 +7216,11 @@
       <c r="H199" s="1">
         <v>75.437978099999995</v>
       </c>
-      <c r="I199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>396</v>
       </c>
@@ -7132,11 +7242,11 @@
       <c r="H200" s="1">
         <v>234.68768299999999</v>
       </c>
-      <c r="I200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>398</v>
       </c>
@@ -7161,11 +7271,11 @@
       <c r="H201" s="1">
         <v>85.133392700000002</v>
       </c>
-      <c r="I201">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>400</v>
       </c>
@@ -7190,11 +7300,11 @@
       <c r="H202" s="1">
         <v>8.8232207999999996</v>
       </c>
-      <c r="I202">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>402</v>
       </c>
@@ -7216,11 +7326,14 @@
       <c r="H203" s="1">
         <v>485.648034</v>
       </c>
-      <c r="I203">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I203" s="2">
+        <v>68.209999084472699</v>
+      </c>
+      <c r="J203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>404</v>
       </c>
@@ -7242,11 +7355,11 @@
       <c r="H204" s="1">
         <v>375.73017599999997</v>
       </c>
-      <c r="I204">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>406</v>
       </c>
@@ -7268,11 +7381,11 @@
       <c r="H205" s="1">
         <v>15.3971722</v>
       </c>
-      <c r="I205">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>408</v>
       </c>
@@ -7292,11 +7405,11 @@
         <v>119.03195599999999</v>
       </c>
       <c r="H206" s="1"/>
-      <c r="I206">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>410</v>
       </c>
@@ -7318,11 +7431,11 @@
       <c r="H207" s="1">
         <v>80.088199200000005</v>
       </c>
-      <c r="I207">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>412</v>
       </c>
@@ -7344,11 +7457,11 @@
       <c r="H208" s="1">
         <v>7915.7304400000003</v>
       </c>
-      <c r="I208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>414</v>
       </c>
@@ -7370,11 +7483,11 @@
       <c r="H209" s="1">
         <v>22.723758499999999</v>
       </c>
-      <c r="I209">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>416</v>
       </c>
@@ -7396,11 +7509,11 @@
       <c r="H210" s="1">
         <v>103.74661999999999</v>
       </c>
-      <c r="I210">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>418</v>
       </c>
@@ -7425,11 +7538,14 @@
       <c r="H211" s="1">
         <v>308.30704600000001</v>
       </c>
-      <c r="I211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I211" s="2">
+        <v>64.209999084472699</v>
+      </c>
+      <c r="J211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>420</v>
       </c>
@@ -7448,11 +7564,11 @@
       <c r="H212" s="1">
         <v>561.18333299999995</v>
       </c>
-      <c r="I212">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>422</v>
       </c>
@@ -7463,11 +7579,11 @@
       <c r="H213" s="1">
         <v>23.255521699999999</v>
       </c>
-      <c r="I213">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>424</v>
       </c>
@@ -7492,11 +7608,14 @@
       <c r="H214" s="1">
         <v>80.2750743</v>
       </c>
-      <c r="I214">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I214" s="2">
+        <v>16.110000610351602</v>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>426</v>
       </c>
@@ -7518,11 +7637,11 @@
       <c r="H215" s="1">
         <v>49.433326600000001</v>
       </c>
-      <c r="I215">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -7531,11 +7650,11 @@
       </c>
       <c r="F216" s="1"/>
       <c r="H216" s="1"/>
-      <c r="I216">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>430</v>
       </c>
@@ -7557,11 +7676,11 @@
       <c r="H217" s="1">
         <v>49.436768000000001</v>
       </c>
-      <c r="I217">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>432</v>
       </c>
@@ -7583,11 +7702,11 @@
       <c r="H218" s="1">
         <v>15.9487811</v>
       </c>
-      <c r="I218">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>434</v>
       </c>
@@ -7612,11 +7731,11 @@
       <c r="H219" s="1">
         <v>215.71770799999999</v>
       </c>
-      <c r="I219">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>436</v>
       </c>
@@ -7638,11 +7757,11 @@
       <c r="H220" s="1">
         <v>3.6570256400000001</v>
       </c>
-      <c r="I220">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>438</v>
       </c>
@@ -7664,11 +7783,11 @@
       <c r="H221" s="1">
         <v>113.12878499999999</v>
       </c>
-      <c r="I221">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>440</v>
       </c>
@@ -7693,11 +7812,11 @@
       <c r="H222" s="1">
         <v>102.59100599999999</v>
       </c>
-      <c r="I222">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>442</v>
       </c>
@@ -7722,11 +7841,11 @@
       <c r="H223" s="1">
         <v>24.692980800000001</v>
       </c>
-      <c r="I223">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>444</v>
       </c>
@@ -7748,11 +7867,11 @@
       <c r="H224" s="1">
         <v>65.3926163</v>
       </c>
-      <c r="I224">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>446</v>
       </c>
@@ -7763,11 +7882,11 @@
       <c r="H225" s="1">
         <v>1193.35294</v>
       </c>
-      <c r="I225">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>448</v>
       </c>
@@ -7789,11 +7908,11 @@
       <c r="H226" s="1">
         <v>208.35434799999999</v>
       </c>
-      <c r="I226">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>450</v>
       </c>
@@ -7804,11 +7923,11 @@
       <c r="H227" s="1">
         <v>92.947786300000004</v>
       </c>
-      <c r="I227">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -7819,11 +7938,11 @@
       <c r="H228" s="1">
         <v>39.068421100000002</v>
       </c>
-      <c r="I228">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>454</v>
       </c>
@@ -7845,11 +7964,11 @@
       <c r="H229" s="1">
         <v>11.925645599999999</v>
       </c>
-      <c r="I229">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>456</v>
       </c>
@@ -7871,11 +7990,11 @@
       <c r="H230" s="1">
         <v>129.33847900000001</v>
       </c>
-      <c r="I230">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>458</v>
       </c>
@@ -7897,11 +8016,11 @@
       <c r="H231" s="1">
         <v>19.918370100000001</v>
       </c>
-      <c r="I231">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>460</v>
       </c>
@@ -7923,11 +8042,14 @@
       <c r="H232" s="1">
         <v>141.542103</v>
       </c>
-      <c r="I232">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I232" s="2">
+        <v>85.169998168945298</v>
+      </c>
+      <c r="J232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>462</v>
       </c>
@@ -7952,11 +8074,14 @@
       <c r="H233" s="1">
         <v>135.46919700000001</v>
       </c>
-      <c r="I233">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I233" s="2">
+        <v>53.150001525878899</v>
+      </c>
+      <c r="J233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -7978,11 +8103,11 @@
       <c r="H234" s="1">
         <v>63.983485799999997</v>
       </c>
-      <c r="I234">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>466</v>
       </c>
@@ -8004,11 +8129,11 @@
       <c r="H235" s="1">
         <v>12.252184400000001</v>
       </c>
-      <c r="I235">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>468</v>
       </c>
@@ -8030,11 +8155,11 @@
       <c r="H236" s="1">
         <v>31.107346100000001</v>
       </c>
-      <c r="I236">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>470</v>
       </c>
@@ -8056,11 +8181,11 @@
       <c r="H237" s="1">
         <v>83.608675199999993</v>
       </c>
-      <c r="I237">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>472</v>
       </c>
@@ -8079,11 +8204,11 @@
       <c r="H238" s="1">
         <v>43.090795499999999</v>
       </c>
-      <c r="I238">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>474</v>
       </c>
@@ -8105,11 +8230,11 @@
       <c r="H239" s="1">
         <v>141.66388900000001</v>
       </c>
-      <c r="I239">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>476</v>
       </c>
@@ -8131,11 +8256,11 @@
       <c r="H240" s="1">
         <v>375.73017599999997</v>
       </c>
-      <c r="I240">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>478</v>
       </c>
@@ -8157,11 +8282,11 @@
       <c r="H241" s="1">
         <v>49.436768000000001</v>
       </c>
-      <c r="I241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>480</v>
       </c>
@@ -8183,11 +8308,11 @@
       <c r="H242" s="1">
         <v>269.79960999999997</v>
       </c>
-      <c r="I242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>482</v>
       </c>
@@ -8209,11 +8334,11 @@
       <c r="H243" s="1">
         <v>73.5932222</v>
       </c>
-      <c r="I243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>484</v>
       </c>
@@ -8238,11 +8363,11 @@
       <c r="H244" s="1">
         <v>105.377769</v>
       </c>
-      <c r="I244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>486</v>
       </c>
@@ -8264,11 +8389,11 @@
       <c r="H245" s="1">
         <v>379</v>
       </c>
-      <c r="I245">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>488</v>
       </c>
@@ -8293,11 +8418,11 @@
       <c r="H246" s="1">
         <v>61.7113412</v>
       </c>
-      <c r="I246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>490</v>
       </c>
@@ -8319,11 +8444,11 @@
       <c r="H247" s="1">
         <v>205.27860100000001</v>
       </c>
-      <c r="I247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>492</v>
       </c>
@@ -8348,11 +8473,11 @@
       <c r="H248" s="1">
         <v>77.389796099999998</v>
       </c>
-      <c r="I248">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>494</v>
       </c>
@@ -8374,11 +8499,11 @@
       <c r="H249" s="1">
         <v>45.153510599999997</v>
       </c>
-      <c r="I249">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>496</v>
       </c>
@@ -8403,11 +8528,14 @@
       <c r="H250" s="1">
         <v>19.635733099999999</v>
       </c>
-      <c r="I250">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I250" s="2">
+        <v>23.639999389648398</v>
+      </c>
+      <c r="J250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>498</v>
       </c>
@@ -8429,11 +8557,11 @@
       <c r="H251" s="1">
         <v>35.545227099999998</v>
       </c>
-      <c r="I251">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>500</v>
       </c>
@@ -8455,11 +8583,11 @@
       <c r="H252" s="1">
         <v>76.136812399999997</v>
       </c>
-      <c r="I252">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>502</v>
       </c>
@@ -8481,11 +8609,11 @@
       <c r="H253" s="1">
         <v>281.60769199999999</v>
       </c>
-      <c r="I253">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>534</v>
       </c>
@@ -8505,11 +8633,14 @@
       <c r="H254" s="1">
         <v>33.3205703</v>
       </c>
-      <c r="I254">
+      <c r="I254" s="2">
+        <v>40</v>
+      </c>
+      <c r="J254">
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>505</v>
       </c>
@@ -8520,11 +8651,11 @@
       <c r="H255" s="1">
         <v>197.18</v>
       </c>
-      <c r="I255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>507</v>
       </c>
@@ -8535,11 +8666,11 @@
       <c r="H256" s="1">
         <v>306.48</v>
       </c>
-      <c r="I256">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>509</v>
       </c>
@@ -8561,11 +8692,14 @@
       <c r="H257" s="1">
         <v>305.081569</v>
       </c>
-      <c r="I257">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I257" s="2">
+        <v>56.060001373291001</v>
+      </c>
+      <c r="J257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>511</v>
       </c>
@@ -8587,11 +8721,11 @@
       <c r="H258" s="1">
         <v>23.421657100000001</v>
       </c>
-      <c r="I258">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>513</v>
       </c>
@@ -8613,11 +8747,11 @@
       <c r="H259" s="1">
         <v>58.9769668</v>
       </c>
-      <c r="I259">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>515</v>
       </c>
@@ -8639,11 +8773,14 @@
       <c r="H260" s="1">
         <v>69.028975299999999</v>
       </c>
-      <c r="I260">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I260" s="2">
+        <v>21.2600002288818</v>
+      </c>
+      <c r="J260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>517</v>
       </c>
@@ -8660,11 +8797,11 @@
       <c r="H261" s="1">
         <v>168.15468000000001</v>
       </c>
-      <c r="I261">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>519</v>
       </c>
@@ -8678,11 +8815,11 @@
       <c r="H262" s="1">
         <v>52.720459499999997</v>
       </c>
-      <c r="I262">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>521</v>
       </c>
@@ -8704,11 +8841,14 @@
       <c r="H263" s="1">
         <v>46.987817100000001</v>
       </c>
-      <c r="I263">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I263" s="2">
+        <v>34.610000610351598</v>
+      </c>
+      <c r="J263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>523</v>
       </c>
@@ -8730,11 +8870,14 @@
       <c r="H264" s="1">
         <v>22.671394599999999</v>
       </c>
-      <c r="I264">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I264" s="2">
+        <v>65.379997253417997</v>
+      </c>
+      <c r="J264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>525</v>
       </c>
@@ -8759,12 +8902,12 @@
       <c r="H265" s="1">
         <v>36.801718999999999</v>
       </c>
-      <c r="I265">
+      <c r="J265">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I265" xr:uid="{DEFDA961-D37F-494B-AAE6-24D3B132EC05}"/>
+  <autoFilter ref="A1:J265" xr:uid="{DEFDA961-D37F-494B-AAE6-24D3B132EC05}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>